<commit_message>
Supplementary Material: Insider Threat Detection using Machine Learning SLR
This repository contains the complete supplementary materials and "audit trail" for our Systematic Literature Review (SLR) on Insider Threat Detection using Machine Learning. This review synthesizes 82 primary studies published between 2021 and 2025.
</commit_message>
<xml_diff>
--- a/02_Study_Selection/Exclusion_Log.xlsx
+++ b/02_Study_Selection/Exclusion_Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rao\Documents\Towards PHD Cyber Security and CNI\Proposals\Journal Submition paper\SLR 2026\SLR-Insider-Threat-Detection-ML-Supplement Alriyami Murthada - Final Copy\02_Study_Selection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rao\Documents\Towards PHD Cyber Security and CNI\Proposals\Journal Submition paper\SLR 2026\SLR-Insider-Threat-Detection-ML-Supplement Alriyami Murtadha - Final Copy\02_Study_Selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEE1A81-4507-4BF8-A365-89FC05E77E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A55BC2B-B9EB-4CEF-8845-E0EF1EAAD56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A5F48124-729C-4F9E-BC95-8219210D1CA7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A5F48124-729C-4F9E-BC95-8219210D1CA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Secondary Studies (Excluded n=1" sheetId="1" r:id="rId1"/>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE5A906-36EF-4DFE-9724-C00510BE8CAB}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -813,7 +813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F7CF7D-F0B0-4EFA-AAA6-EE93F9101F65}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>

</xml_diff>